<commit_message>
new folder structure, corrected ad-png-files
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\OneDrive\Dokumente\Studium\Abschlussprojekt\4_Entwurf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\OneDrive\Dokumente\Studium\Abschlussprojekt\GitHub_Repository\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E43232-C708-40BE-A2C8-2E6BE7DA3557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94962CEE-CDC9-4270-B701-DF1B6481D45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24345" yWindow="2565" windowWidth="21630" windowHeight="11250" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
+    <workbookView xWindow="-25710" yWindow="-1880" windowWidth="25820" windowHeight="13900" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>das endgültige Entfernen von Daten aus einem Speichersystem, nach welchem die Daten nicht wiederherstellbar sind</t>
+  </si>
+  <si>
+    <t>auswählen</t>
+  </si>
+  <si>
+    <t>das Selektieren einer dargebotenen Option auf der Nutzeroberfläche</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,9 +194,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -527,15 +530,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" style="5" customWidth="1"/>
+    <col min="1" max="1" width="18" style="4" customWidth="1"/>
     <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
   </cols>
@@ -552,7 +555,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -560,7 +563,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -569,7 +572,7 @@
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -577,7 +580,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -586,7 +589,7 @@
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -595,7 +598,7 @@
       <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -604,7 +607,7 @@
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -613,7 +616,7 @@
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -622,7 +625,7 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -630,7 +633,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -638,7 +641,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -647,7 +650,7 @@
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -655,7 +658,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -663,7 +666,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -671,11 +674,19 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in folder structure, moved some files, renamed domain class diagram draw.io-file, added new process words to table of defined process words
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\OneDrive\Dokumente\Studium\Abschlussprojekt\GitHub_Repository\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94962CEE-CDC9-4270-B701-DF1B6481D45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE051CC3-1B30-46FF-8F89-673BB69E333C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25710" yWindow="-1880" windowWidth="25820" windowHeight="13900" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Semantische Definition</t>
   </si>
   <si>
-    <t>Synonyme</t>
-  </si>
-  <si>
     <t>anzeigen</t>
   </si>
   <si>
@@ -141,6 +138,12 @@
   </si>
   <si>
     <t>das Selektieren einer dargebotenen Option auf der Nutzeroberfläche</t>
+  </si>
+  <si>
+    <t>bearbeiten</t>
+  </si>
+  <si>
+    <t>das Verändern von existierenden Daten, Objekten,  Eigenschaften oder Verbindungen</t>
   </si>
 </sst>
 </file>
@@ -530,17 +533,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="4" customWidth="1"/>
     <col min="2" max="2" width="39.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -550,148 +553,154 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>34</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
-    <sortCondition ref="A1:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+    <sortCondition ref="A5:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added new process word to table of defined process words
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\OneDrive\Dokumente\Studium\Abschlussprojekt\GitHub_Repository\4_Entwurf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE051CC3-1B30-46FF-8F89-673BB69E333C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D1995D-A5D4-4BB8-A74D-DB3D0A34D912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25710" yWindow="-1880" windowWidth="25820" windowHeight="13900" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>das Verändern von existierenden Daten, Objekten,  Eigenschaften oder Verbindungen</t>
+  </si>
+  <si>
+    <t>markieren</t>
+  </si>
+  <si>
+    <t>das Selektieren einer dargebotenen Option auf der Nutzeroberfläche durch optische Hervorhebung</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +561,7 @@
       </c>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>22</v>
       </c>
@@ -572,7 +578,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
@@ -580,7 +586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
@@ -613,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -631,7 +637,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
@@ -640,7 +646,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
@@ -667,40 +673,48 @@
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
-    <sortCondition ref="A5:A18"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
+    <sortCondition ref="A14:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added words to table of defined process words, added requirements to table of functional requirements, transferred requirements to LaTeX-table (to be uploadet later: enhanced, updated, sorted, many additions)
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D1995D-A5D4-4BB8-A74D-DB3D0A34D912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445CF7C4-22E6-4775-B292-1DA264B956B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -86,12 +86,6 @@
     <t>das Erstellen einer Verbindung zwischen Daten oder Objekten</t>
   </si>
   <si>
-    <t>modifizieren</t>
-  </si>
-  <si>
-    <t>nachträgliche strukturelle oder inhaltliche Änderung von Daten, Objekten oder Verbindungen durch die Nutzer*in</t>
-  </si>
-  <si>
     <t>bestätigen</t>
   </si>
   <si>
@@ -150,6 +144,27 @@
   </si>
   <si>
     <t>das Selektieren einer dargebotenen Option auf der Nutzeroberfläche durch optische Hervorhebung</t>
+  </si>
+  <si>
+    <t>aktivieren</t>
+  </si>
+  <si>
+    <t>deaktivieren</t>
+  </si>
+  <si>
+    <t>priorisieren</t>
+  </si>
+  <si>
+    <t>behandeln</t>
+  </si>
+  <si>
+    <t>ignorieren</t>
+  </si>
+  <si>
+    <t>pausieren</t>
+  </si>
+  <si>
+    <t>fortsetzen</t>
   </si>
 </sst>
 </file>
@@ -539,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,10 +578,10 @@
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -574,40 +589,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="4"/>
     </row>
@@ -621,10 +636,10 @@
     </row>
     <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="C9" s="4"/>
     </row>
@@ -642,7 +657,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="4"/>
     </row>
@@ -665,56 +680,82 @@
     </row>
     <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>15</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B19">
-    <sortCondition ref="A14:A19"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+    <sortCondition ref="A14:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added process words and ressources on ableism
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Assistenz_Dienstplaner\GitHub_Repository\4_Entwurf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\Praxisprojekt_AssistenzDienstplaner\GitRepository\praxisprojekt_mi_bachelor_SoSe24\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445CF7C4-22E6-4775-B292-1DA264B956B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64885BA-D5FA-4506-BB2F-70116C430157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>fortsetzen</t>
+  </si>
+  <si>
+    <t>einlesen</t>
+  </si>
+  <si>
+    <t>zulassen</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,6 +759,16 @@
         <v>42</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
     <sortCondition ref="A14:A18"/>

</xml_diff>

<commit_message>
added textual specification, updated tables
</commit_message>
<xml_diff>
--- a/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
+++ b/4_Entwurf/4_DefinitionenDerProzesswörter.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alenn\Praxisprojekt_AssistenzDienstplaner\GitRepository\praxisprojekt_mi_bachelor_SoSe24\4_Entwurf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64885BA-D5FA-4506-BB2F-70116C430157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6358DCD-D348-4108-9FD0-4FE811B17412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EE0CB38E-DD33-4E08-8A12-56D45FDECCAA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Prozesswort</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>zulassen</t>
+  </si>
+  <si>
+    <t>verwalten</t>
   </si>
 </sst>
 </file>
@@ -560,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462FDA02-6416-444E-A84A-3DB1F36ADCB5}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,6 +772,11 @@
         <v>44</v>
       </c>
     </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
     <sortCondition ref="A14:A18"/>

</xml_diff>